<commit_message>
Update for new excell form 2021. refactoring
</commit_message>
<xml_diff>
--- a/Excell/zhr_svarki.xlsx
+++ b/Excell/zhr_svarki.xlsx
@@ -16,7 +16,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Context!$A$1:$AT$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Tittle!$A$1:$AQ$48</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -81,9 +81,6 @@
     <t>на участке</t>
   </si>
   <si>
-    <t xml:space="preserve">на МНПП </t>
-  </si>
-  <si>
     <t>от км/ПК</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
   </si>
   <si>
     <t>12.12.2020 г.</t>
-  </si>
-  <si>
-    <t>zdsadasda</t>
   </si>
   <si>
     <t>Начало</t>
@@ -211,6 +205,12 @@
   </si>
   <si>
     <t>Продолжение</t>
+  </si>
+  <si>
+    <t>на трассе</t>
+  </si>
+  <si>
+    <t>СЗСМ</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -675,6 +675,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -683,21 +686,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -718,16 +706,35 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1033,8 +1040,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:AX152"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="AN12" sqref="AN12"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A25" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="AK30" sqref="AK30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1320,11 +1327,11 @@
       <c r="S11" s="25"/>
       <c r="T11" s="25"/>
       <c r="U11" s="25"/>
-      <c r="V11" s="25"/>
+      <c r="V11" s="76" t="s">
+        <v>58</v>
+      </c>
       <c r="W11" s="26"/>
-      <c r="X11" s="27" t="s">
-        <v>19</v>
-      </c>
+      <c r="X11" s="27"/>
       <c r="Y11" s="25"/>
       <c r="Z11" s="25"/>
       <c r="AA11" s="25"/>
@@ -1374,7 +1381,7 @@
       <c r="O13" s="12"/>
       <c r="P13" s="28"/>
       <c r="Q13" s="29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R13" s="28"/>
       <c r="S13" s="57"/>
@@ -1383,7 +1390,7 @@
       <c r="V13" s="57"/>
       <c r="W13" s="30"/>
       <c r="X13" s="31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Y13" s="28"/>
       <c r="Z13" s="32"/>
@@ -1607,7 +1614,7 @@
     </row>
     <row r="18" spans="1:47" ht="15" customHeight="1">
       <c r="A18" s="34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="33"/>
@@ -1628,9 +1635,7 @@
       <c r="R18" s="35"/>
       <c r="S18" s="35"/>
       <c r="T18" s="35"/>
-      <c r="U18" s="35" t="s">
-        <v>29</v>
-      </c>
+      <c r="U18" s="35"/>
       <c r="V18" s="35"/>
       <c r="W18" s="35"/>
       <c r="X18" s="35"/>
@@ -1661,13 +1666,13 @@
     <row r="19" spans="1:47">
       <c r="A19" s="34"/>
       <c r="U19" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF19" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AF19" s="36" t="s">
+      <c r="AM19" s="36" t="s">
         <v>24</v>
-      </c>
-      <c r="AM19" s="36" t="s">
-        <v>25</v>
       </c>
       <c r="AR19" s="13"/>
       <c r="AS19" s="13"/>
@@ -1689,10 +1694,10 @@
     </row>
     <row r="23" spans="1:47">
       <c r="AK23" s="37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AL23" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AM23" s="6"/>
       <c r="AN23" s="37"/>
@@ -1700,10 +1705,10 @@
     </row>
     <row r="25" spans="1:47">
       <c r="AK25" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL25" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="AL25" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="AM25" s="6"/>
       <c r="AN25" s="37"/>
@@ -2230,26 +2235,26 @@
       <c r="U43" s="14"/>
       <c r="V43" s="14"/>
       <c r="W43" s="14"/>
-      <c r="X43" s="14"/>
-      <c r="Y43" s="14"/>
-      <c r="Z43" s="14"/>
-      <c r="AA43" s="14"/>
-      <c r="AB43" s="14"/>
-      <c r="AC43" s="14"/>
-      <c r="AD43" s="14"/>
-      <c r="AE43" s="14"/>
-      <c r="AF43" s="14"/>
-      <c r="AG43" s="14"/>
-      <c r="AH43" s="14"/>
-      <c r="AI43" s="14"/>
-      <c r="AJ43" s="14"/>
-      <c r="AK43" s="14"/>
-      <c r="AL43" s="14"/>
-      <c r="AM43" s="14"/>
-      <c r="AN43" s="14"/>
-      <c r="AO43" s="14"/>
-      <c r="AP43" s="14"/>
-      <c r="AQ43" s="14"/>
+      <c r="X43" s="77"/>
+      <c r="Y43" s="77"/>
+      <c r="Z43" s="77"/>
+      <c r="AA43" s="77"/>
+      <c r="AB43" s="77"/>
+      <c r="AC43" s="77"/>
+      <c r="AD43" s="77"/>
+      <c r="AE43" s="77"/>
+      <c r="AF43" s="77"/>
+      <c r="AG43" s="77"/>
+      <c r="AH43" s="77"/>
+      <c r="AI43" s="77"/>
+      <c r="AJ43" s="77"/>
+      <c r="AK43" s="77"/>
+      <c r="AL43" s="77"/>
+      <c r="AM43" s="77"/>
+      <c r="AN43" s="77"/>
+      <c r="AO43" s="77"/>
+      <c r="AP43" s="77"/>
+      <c r="AQ43" s="77"/>
       <c r="AR43" s="14"/>
       <c r="AS43" s="14"/>
     </row>
@@ -2277,26 +2282,26 @@
       <c r="U44" s="14"/>
       <c r="V44" s="14"/>
       <c r="W44" s="14"/>
-      <c r="X44" s="14"/>
-      <c r="Y44" s="14"/>
-      <c r="Z44" s="14"/>
-      <c r="AA44" s="14"/>
-      <c r="AB44" s="14"/>
-      <c r="AC44" s="14"/>
-      <c r="AD44" s="14"/>
-      <c r="AE44" s="14"/>
-      <c r="AF44" s="14"/>
-      <c r="AG44" s="14"/>
-      <c r="AH44" s="14"/>
-      <c r="AI44" s="14"/>
-      <c r="AJ44" s="14"/>
-      <c r="AK44" s="14"/>
-      <c r="AL44" s="14"/>
-      <c r="AM44" s="14"/>
-      <c r="AN44" s="14"/>
-      <c r="AO44" s="14"/>
-      <c r="AP44" s="14"/>
-      <c r="AQ44" s="14"/>
+      <c r="X44" s="77"/>
+      <c r="Y44" s="77"/>
+      <c r="Z44" s="77"/>
+      <c r="AA44" s="77"/>
+      <c r="AB44" s="77"/>
+      <c r="AC44" s="77"/>
+      <c r="AD44" s="77"/>
+      <c r="AE44" s="77"/>
+      <c r="AF44" s="77"/>
+      <c r="AG44" s="77"/>
+      <c r="AH44" s="77"/>
+      <c r="AI44" s="77"/>
+      <c r="AJ44" s="77"/>
+      <c r="AK44" s="77"/>
+      <c r="AL44" s="77"/>
+      <c r="AM44" s="77"/>
+      <c r="AN44" s="77"/>
+      <c r="AO44" s="77"/>
+      <c r="AP44" s="77"/>
+      <c r="AQ44" s="77"/>
       <c r="AR44" s="14"/>
       <c r="AS44" s="14"/>
     </row>
@@ -2324,26 +2329,26 @@
       <c r="U45" s="14"/>
       <c r="V45" s="14"/>
       <c r="W45" s="14"/>
-      <c r="X45" s="14"/>
-      <c r="Y45" s="14"/>
-      <c r="Z45" s="14"/>
-      <c r="AA45" s="14"/>
-      <c r="AB45" s="14"/>
-      <c r="AC45" s="14"/>
-      <c r="AD45" s="14"/>
-      <c r="AE45" s="14"/>
-      <c r="AF45" s="14"/>
-      <c r="AG45" s="14"/>
-      <c r="AH45" s="14"/>
-      <c r="AI45" s="14"/>
-      <c r="AJ45" s="14"/>
-      <c r="AK45" s="14"/>
-      <c r="AL45" s="14"/>
-      <c r="AM45" s="14"/>
-      <c r="AN45" s="14"/>
-      <c r="AO45" s="14"/>
-      <c r="AP45" s="14"/>
-      <c r="AQ45" s="14"/>
+      <c r="X45" s="77"/>
+      <c r="Y45" s="77"/>
+      <c r="Z45" s="77"/>
+      <c r="AA45" s="77"/>
+      <c r="AB45" s="77"/>
+      <c r="AC45" s="77"/>
+      <c r="AD45" s="77"/>
+      <c r="AE45" s="77"/>
+      <c r="AF45" s="77"/>
+      <c r="AG45" s="77"/>
+      <c r="AH45" s="77"/>
+      <c r="AI45" s="77"/>
+      <c r="AJ45" s="77"/>
+      <c r="AK45" s="77"/>
+      <c r="AL45" s="77"/>
+      <c r="AM45" s="77"/>
+      <c r="AN45" s="77"/>
+      <c r="AO45" s="77"/>
+      <c r="AP45" s="77"/>
+      <c r="AQ45" s="77"/>
       <c r="AR45" s="14"/>
       <c r="AS45" s="14"/>
     </row>
@@ -2371,26 +2376,26 @@
       <c r="U46" s="14"/>
       <c r="V46" s="14"/>
       <c r="W46" s="14"/>
-      <c r="X46" s="14"/>
-      <c r="Y46" s="14"/>
-      <c r="Z46" s="14"/>
-      <c r="AA46" s="14"/>
-      <c r="AB46" s="14"/>
-      <c r="AC46" s="14"/>
-      <c r="AD46" s="14"/>
-      <c r="AE46" s="14"/>
-      <c r="AF46" s="14"/>
-      <c r="AG46" s="14"/>
-      <c r="AH46" s="14"/>
-      <c r="AI46" s="14"/>
-      <c r="AJ46" s="14"/>
-      <c r="AK46" s="14"/>
-      <c r="AL46" s="14"/>
-      <c r="AM46" s="14"/>
-      <c r="AN46" s="14"/>
-      <c r="AO46" s="14"/>
-      <c r="AP46" s="14"/>
-      <c r="AQ46" s="14"/>
+      <c r="X46" s="77"/>
+      <c r="Y46" s="77"/>
+      <c r="Z46" s="77"/>
+      <c r="AA46" s="77"/>
+      <c r="AB46" s="77"/>
+      <c r="AC46" s="77"/>
+      <c r="AD46" s="77"/>
+      <c r="AE46" s="77"/>
+      <c r="AF46" s="77"/>
+      <c r="AG46" s="77"/>
+      <c r="AH46" s="77"/>
+      <c r="AI46" s="77"/>
+      <c r="AJ46" s="77"/>
+      <c r="AK46" s="77"/>
+      <c r="AL46" s="77"/>
+      <c r="AM46" s="77"/>
+      <c r="AN46" s="77"/>
+      <c r="AO46" s="77"/>
+      <c r="AP46" s="78"/>
+      <c r="AQ46" s="77"/>
       <c r="AR46" s="14"/>
       <c r="AS46" s="14"/>
     </row>
@@ -2418,26 +2423,26 @@
       <c r="U47" s="14"/>
       <c r="V47" s="14"/>
       <c r="W47" s="14"/>
-      <c r="X47" s="14"/>
-      <c r="Y47" s="14"/>
-      <c r="Z47" s="14"/>
-      <c r="AA47" s="14"/>
-      <c r="AB47" s="14"/>
-      <c r="AC47" s="14"/>
-      <c r="AD47" s="14"/>
-      <c r="AE47" s="14"/>
-      <c r="AF47" s="14"/>
-      <c r="AG47" s="14"/>
-      <c r="AH47" s="14"/>
-      <c r="AI47" s="14"/>
-      <c r="AJ47" s="14"/>
-      <c r="AK47" s="14"/>
-      <c r="AL47" s="14"/>
-      <c r="AM47" s="14"/>
-      <c r="AN47" s="14"/>
-      <c r="AO47" s="14"/>
-      <c r="AP47" s="14"/>
-      <c r="AQ47" s="14"/>
+      <c r="X47" s="77"/>
+      <c r="Y47" s="77"/>
+      <c r="Z47" s="77"/>
+      <c r="AA47" s="77"/>
+      <c r="AB47" s="77"/>
+      <c r="AC47" s="77"/>
+      <c r="AD47" s="77"/>
+      <c r="AE47" s="77"/>
+      <c r="AF47" s="77"/>
+      <c r="AG47" s="77"/>
+      <c r="AH47" s="77"/>
+      <c r="AI47" s="77"/>
+      <c r="AJ47" s="77"/>
+      <c r="AK47" s="77"/>
+      <c r="AL47" s="77"/>
+      <c r="AM47" s="77"/>
+      <c r="AN47" s="77"/>
+      <c r="AO47" s="77"/>
+      <c r="AP47" s="78"/>
+      <c r="AQ47" s="77"/>
       <c r="AR47" s="14"/>
       <c r="AS47" s="14"/>
     </row>
@@ -2465,26 +2470,26 @@
       <c r="U48" s="14"/>
       <c r="V48" s="14"/>
       <c r="W48" s="14"/>
-      <c r="X48" s="14"/>
-      <c r="Y48" s="14"/>
-      <c r="Z48" s="14"/>
-      <c r="AA48" s="14"/>
-      <c r="AB48" s="14"/>
-      <c r="AC48" s="14"/>
-      <c r="AD48" s="14"/>
-      <c r="AE48" s="14"/>
-      <c r="AF48" s="14"/>
-      <c r="AG48" s="14"/>
-      <c r="AH48" s="14"/>
-      <c r="AI48" s="14"/>
-      <c r="AJ48" s="14"/>
-      <c r="AK48" s="14"/>
-      <c r="AL48" s="14"/>
-      <c r="AM48" s="14"/>
-      <c r="AN48" s="14"/>
-      <c r="AO48" s="14"/>
-      <c r="AP48" s="14"/>
-      <c r="AQ48" s="14"/>
+      <c r="X48" s="77"/>
+      <c r="Y48" s="77"/>
+      <c r="Z48" s="77"/>
+      <c r="AA48" s="77"/>
+      <c r="AB48" s="77"/>
+      <c r="AC48" s="77"/>
+      <c r="AD48" s="77"/>
+      <c r="AE48" s="77"/>
+      <c r="AF48" s="77"/>
+      <c r="AG48" s="77"/>
+      <c r="AH48" s="77"/>
+      <c r="AI48" s="77"/>
+      <c r="AJ48" s="77"/>
+      <c r="AK48" s="77"/>
+      <c r="AL48" s="77"/>
+      <c r="AM48" s="77"/>
+      <c r="AN48" s="77"/>
+      <c r="AO48" s="77"/>
+      <c r="AP48" s="77"/>
+      <c r="AQ48" s="77"/>
       <c r="AR48" s="14"/>
       <c r="AS48" s="14"/>
     </row>
@@ -7164,32 +7169,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT49"/>
+  <dimension ref="A1:AU49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="AH17" sqref="AH17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="3" style="5" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="5" customWidth="1"/>
     <col min="3" max="4" width="4.85546875" style="5" customWidth="1"/>
-    <col min="5" max="6" width="5.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="5" customWidth="1"/>
     <col min="7" max="7" width="4.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="9" style="5" customWidth="1"/>
-    <col min="9" max="10" width="4.85546875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="4.5703125" style="5" customWidth="1"/>
-    <col min="12" max="13" width="4.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8" style="5" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="6" style="5" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="3.42578125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="7" style="5" customWidth="1"/>
     <col min="14" max="14" width="4.28515625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="4" style="5" customWidth="1"/>
+    <col min="15" max="15" width="3.7109375" style="5" customWidth="1"/>
     <col min="16" max="16" width="4.140625" style="5" customWidth="1"/>
     <col min="17" max="17" width="4.28515625" style="5" customWidth="1"/>
     <col min="18" max="18" width="8" style="5" customWidth="1"/>
     <col min="19" max="19" width="4.85546875" style="5" customWidth="1"/>
     <col min="20" max="20" width="5.7109375" style="5" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" style="5" customWidth="1"/>
-    <col min="22" max="23" width="6.42578125" style="5" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" style="5" customWidth="1"/>
+    <col min="22" max="22" width="6.42578125" style="5" customWidth="1"/>
+    <col min="23" max="23" width="5.5703125" style="5" customWidth="1"/>
     <col min="24" max="24" width="4.85546875" style="5" customWidth="1"/>
     <col min="25" max="25" width="12.140625" style="5" customWidth="1"/>
     <col min="26" max="26" width="6.85546875" style="5" customWidth="1"/>
@@ -7213,275 +7222,278 @@
     <col min="47" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46">
+    <row r="1" spans="1:47">
       <c r="A1" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU1" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" ht="10.5" customHeight="1">
+      <c r="A2" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:46" ht="10.5" customHeight="1">
-      <c r="A2" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="58" t="s">
+      <c r="D2" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="E2" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="F2" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="G2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="J2" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="58" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="66" t="s">
+      <c r="K2" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="63"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="67"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="72" t="s">
+      <c r="O2" s="68"/>
+      <c r="P2" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="59" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="73"/>
-      <c r="P2" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" s="58" t="s">
+      <c r="T2" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="58" t="s">
+      <c r="U2" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="U2" s="72" t="s">
-        <v>47</v>
-      </c>
-      <c r="V2" s="72"/>
-      <c r="W2" s="72"/>
-      <c r="X2" s="72" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" s="72"/>
-      <c r="Z2" s="72"/>
-      <c r="AA2" s="72"/>
-      <c r="AB2" s="72"/>
-      <c r="AC2" s="72"/>
-      <c r="AD2" s="72"/>
-      <c r="AE2" s="72"/>
-      <c r="AF2" s="66" t="s">
-        <v>54</v>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="58"/>
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="62" t="s">
+        <v>52</v>
       </c>
       <c r="AG2" s="74"/>
       <c r="AH2" s="75"/>
-      <c r="AI2" s="63" t="s">
+      <c r="AI2" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ2" s="72"/>
+      <c r="AK2" s="72"/>
+      <c r="AL2" s="72"/>
+      <c r="AM2" s="72"/>
+      <c r="AN2" s="72"/>
+      <c r="AO2" s="72"/>
+      <c r="AP2" s="72"/>
+      <c r="AQ2" s="72"/>
+      <c r="AR2" s="72"/>
+      <c r="AS2" s="72"/>
+      <c r="AT2" s="59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" ht="27.75" customHeight="1">
+      <c r="A3" s="60"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58"/>
+      <c r="AF3" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG3" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH3" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI3" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="AJ2" s="64"/>
-      <c r="AK2" s="64"/>
-      <c r="AL2" s="64"/>
-      <c r="AM2" s="64"/>
-      <c r="AN2" s="64"/>
-      <c r="AO2" s="64"/>
-      <c r="AP2" s="64"/>
-      <c r="AQ2" s="64"/>
-      <c r="AR2" s="64"/>
-      <c r="AS2" s="64"/>
-      <c r="AT2" s="58" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:46" ht="27.75" customHeight="1">
-      <c r="A3" s="59"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
-      <c r="R3" s="59"/>
-      <c r="S3" s="59"/>
-      <c r="T3" s="59"/>
-      <c r="U3" s="72" t="s">
+      <c r="AJ3" s="72"/>
+      <c r="AK3" s="73"/>
+      <c r="AL3" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM3" s="72"/>
+      <c r="AN3" s="72"/>
+      <c r="AO3" s="73"/>
+      <c r="AP3" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ3" s="72"/>
+      <c r="AR3" s="72"/>
+      <c r="AS3" s="72"/>
+      <c r="AT3" s="60"/>
+    </row>
+    <row r="4" spans="1:47" ht="53.25" customHeight="1">
+      <c r="A4" s="61"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="61"/>
+      <c r="U4" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="V4" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="W4" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="X4" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="V3" s="72"/>
-      <c r="W3" s="72"/>
-      <c r="X3" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y3" s="72"/>
-      <c r="Z3" s="72"/>
-      <c r="AA3" s="72"/>
-      <c r="AB3" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC3" s="72"/>
-      <c r="AD3" s="72"/>
-      <c r="AE3" s="72"/>
-      <c r="AF3" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG3" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH3" s="61" t="s">
-        <v>6</v>
-      </c>
-      <c r="AI3" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ3" s="64"/>
-      <c r="AK3" s="65"/>
-      <c r="AL3" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="59"/>
-    </row>
-    <row r="4" spans="1:46" ht="53.25" customHeight="1">
-      <c r="A4" s="60"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="60"/>
-      <c r="S4" s="60"/>
-      <c r="T4" s="60"/>
-      <c r="U4" s="48" t="s">
+      <c r="Y4" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z4" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA4" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="W4" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="X4" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y4" s="48" t="s">
+      <c r="AB4" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC4" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD4" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE4" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="Z4" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA4" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB4" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC4" s="48" t="s">
+      <c r="AF4" s="61"/>
+      <c r="AG4" s="61"/>
+      <c r="AH4" s="70"/>
+      <c r="AI4" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ4" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK4" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="AD4" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE4" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF4" s="60"/>
-      <c r="AG4" s="60"/>
-      <c r="AH4" s="62"/>
-      <c r="AI4" s="48" t="s">
+      <c r="AL4" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM4" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="AN4" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO4" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="AJ4" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="AK4" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL4" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM4" s="48" t="s">
+      <c r="AP4" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ4" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR4" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="AS4" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="AN4" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="AO4" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP4" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ4" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="AR4" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="AS4" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AT4" s="60"/>
-    </row>
-    <row r="5" spans="1:46">
+      <c r="AT4" s="61"/>
+    </row>
+    <row r="5" spans="1:47">
       <c r="A5" s="16">
         <v>1</v>
       </c>
@@ -7621,46 +7633,46 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:46" s="40" customFormat="1" ht="19.5" customHeight="1">
+    <row r="6" spans="1:47" s="40" customFormat="1" ht="19.5" customHeight="1">
       <c r="B6" s="41"/>
     </row>
-    <row r="7" spans="1:46" ht="19.5" customHeight="1">
+    <row r="7" spans="1:47" ht="19.5" customHeight="1">
       <c r="H7" s="40"/>
       <c r="AC7" s="40"/>
     </row>
-    <row r="8" spans="1:46">
+    <row r="8" spans="1:47">
       <c r="H8" s="40"/>
       <c r="AC8" s="40"/>
     </row>
-    <row r="9" spans="1:46">
+    <row r="9" spans="1:47">
       <c r="H9" s="40"/>
       <c r="AC9" s="40"/>
     </row>
-    <row r="10" spans="1:46">
+    <row r="10" spans="1:47">
       <c r="H10" s="40"/>
       <c r="AC10" s="40"/>
     </row>
-    <row r="11" spans="1:46">
+    <row r="11" spans="1:47">
       <c r="H11" s="40"/>
       <c r="AC11" s="40"/>
     </row>
-    <row r="12" spans="1:46">
+    <row r="12" spans="1:47">
       <c r="H12" s="40"/>
       <c r="AC12" s="40"/>
     </row>
-    <row r="13" spans="1:46">
+    <row r="13" spans="1:47">
       <c r="H13" s="40"/>
       <c r="AC13" s="40"/>
     </row>
-    <row r="14" spans="1:46">
+    <row r="14" spans="1:47">
       <c r="H14" s="40"/>
       <c r="AC14" s="40"/>
     </row>
-    <row r="15" spans="1:46">
+    <row r="15" spans="1:47">
       <c r="H15" s="40"/>
       <c r="AC15" s="40"/>
     </row>
-    <row r="16" spans="1:46">
+    <row r="16" spans="1:47">
       <c r="H16" s="40"/>
       <c r="AC16" s="40"/>
     </row>
@@ -7800,28 +7812,6 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="31">
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="X2:AE2"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="P2:P4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:M3"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="S2:S4"/>
-    <mergeCell ref="T2:T4"/>
-    <mergeCell ref="X3:AA3"/>
-    <mergeCell ref="AB3:AE3"/>
-    <mergeCell ref="R2:R4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
     <mergeCell ref="AT2:AT4"/>
     <mergeCell ref="AF3:AF4"/>
     <mergeCell ref="AG3:AG4"/>
@@ -7831,6 +7821,28 @@
     <mergeCell ref="AL3:AO3"/>
     <mergeCell ref="AP3:AS3"/>
     <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:M3"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="S2:S4"/>
+    <mergeCell ref="T2:T4"/>
+    <mergeCell ref="R2:R4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="X2:AE2"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="X3:AA3"/>
+    <mergeCell ref="AB3:AE3"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>